<commit_message>
added latest DR update
</commit_message>
<xml_diff>
--- a/Backend/historic/hist_DR.xlsx
+++ b/Backend/historic/hist_DR.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1024,9 +1024,23 @@
         <v>4716632ceb622629977f4fc5e727772ff5c8d972ba3dfb804d923198a2aa2bc3</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="str">
+        <v>04.08.2023 12:31 (CET)</v>
+      </c>
+      <c r="C47" t="str">
+        <v>{"ProposedVersion":"https://github.com/tibonto/dr/commit/85f9cce24c27847fce2b2bb1ee7d9f2e05ce802d ","UpdatedVersion":"https://github.com/tibonto/dr/commit/85f9cce24c27847fce2b2bb1ee7d9f2e05ce802d","Domain":"Planning","LobeOwner":"member1","Result":"accept by lobe owner"}</v>
+      </c>
+      <c r="D47" t="str">
+        <v>4a51a8bbb1a7b315d67ec715f9a71e4197aedf566442f359dff5013557f046c7</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D46"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D47"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>